<commit_message>
niewielkie zmiany w opisie moga... do sprawdzenia (część wywalona)
</commit_message>
<xml_diff>
--- a/doc/wyniki.xlsx
+++ b/doc/wyniki.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="53">
   <si>
     <t>clip01</t>
   </si>
@@ -607,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -669,6 +669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -708,2011 +709,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="300">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="100">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -4138,6 +2151,25 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Sekwencja</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4156,7 +2188,26 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Błąd średniokwadratowy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4166,7 +2217,7 @@
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -5473,10 +3524,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="134"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="34"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -6106,6 +4157,25 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Sekwencja</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6124,6 +4194,25 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Błąd średniokwadratowy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -6134,7 +4223,7 @@
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -6790,6 +4879,25 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Sekwencja</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6808,6 +4916,30 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Błąd</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> średniokwadratowy</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -6818,7 +4950,7 @@
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -6860,11 +4992,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$229</c:f>
+              <c:f>Sheet1!$O$57:$O$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Średnia</c:v>
+                  <c:v>Metoda Mediana</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6872,7 +5004,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$228:$I$228</c:f>
+              <c:f>Sheet1!$N$59:$N$65</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -6901,30 +5033,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$229:$I$229</c:f>
+              <c:f>Sheet1!$O$59:$O$65</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>85.9989474508303</c:v>
+                  <c:v>53.892113710105299</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.393422872502398</c:v>
+                  <c:v>13.1535982393723</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>198.54944371471601</c:v>
+                  <c:v>201.54178446228701</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62.8719152045512</c:v>
+                  <c:v>32.724114684365702</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.753714622641503</c:v>
+                  <c:v>36.534389740565999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56.498554687499997</c:v>
+                  <c:v>52.789596354166697</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>105.04234722222201</c:v>
+                  <c:v>24.915791666666699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6935,11 +5067,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$230</c:f>
+              <c:f>Sheet1!$P$57:$P$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Mediana</c:v>
+                  <c:v>Metoda MOG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6947,7 +5079,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$228:$I$228</c:f>
+              <c:f>Sheet1!$N$59:$N$65</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -6976,82 +5108,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$230:$I$230</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>53.892113710105299</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.1535982393723</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>201.54178446228701</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32.724114684365702</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>36.534389740565999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>52.789596354166697</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24.915791666666699</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$231</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MOG</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$228:$I$228</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>clip_01.mpg</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>clip_02.mpg</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>clip_03.mpg</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>clip_04.mpg</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>fountain.mpg</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>highway.mpg</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>pedestrians.mpg</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$231:$I$231</c:f>
+              <c:f>Sheet1!$P$59:$P$65</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -7075,231 +5132,6 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>33.341111111111097</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$232</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Aproksymacja średniej</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$228:$I$228</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>clip_01.mpg</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>clip_02.mpg</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>clip_03.mpg</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>clip_04.mpg</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>fountain.mpg</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>highway.mpg</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>pedestrians.mpg</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$232:$I$232</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>64.549156655851206</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29.543028384032599</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>151.619960159709</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21.694773788916098</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13.092158018867901</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>71.376106770833303</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>67.848944444444399</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$233</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>DCT</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$228:$I$228</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>clip_01.mpg</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>clip_02.mpg</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>clip_03.mpg</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>clip_04.mpg</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>fountain.mpg</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>highway.mpg</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>pedestrians.mpg</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$233:$I$233</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>43.188145338772998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>37.526083212275701</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>183.35071634234799</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34.174657921519803</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>70.76953125</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>47.315195312500002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>84.560569444444397</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$234</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Hadamard</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$228:$I$228</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>clip_01.mpg</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>clip_02.mpg</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>clip_03.mpg</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>clip_04.mpg</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>fountain.mpg</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>highway.mpg</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>pedestrians.mpg</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$234:$I$234</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>43.186792682608598</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>37.505075722649003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>183.34579284788501</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34.360867787646001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>70.773565779999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>47.859283854166698</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>84.545694444444507</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7314,20 +5146,39 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="155653632"/>
-        <c:axId val="155702400"/>
+        <c:axId val="120008064"/>
+        <c:axId val="120128640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="155653632"/>
+        <c:axId val="120008064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sekwencja</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155702400"/>
+        <c:crossAx val="120128640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7335,24 +5186,43 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="155702400"/>
+        <c:axId val="120128640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Błąd średniokwadratowy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155653632"/>
+        <c:crossAx val="120008064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -7394,11 +5264,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$57:$O$58</c:f>
+              <c:f>Sheet1!$C$253:$C$254</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Metoda Mediana</c:v>
+                  <c:v>Metoda MOG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7406,7 +5276,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$N$59:$N$65</c:f>
+              <c:f>Sheet1!$B$255:$B$261</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -7435,30 +5305,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$59:$O$65</c:f>
+              <c:f>Sheet1!$C$255:$C$261</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>53.892113710105299</c:v>
+                  <c:v>86.263981071512504</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.1535982393723</c:v>
+                  <c:v>25.1932602058125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>201.54178446228701</c:v>
+                  <c:v>181.01076035804101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.724114684365702</c:v>
+                  <c:v>63.4836854878696</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.534389740565999</c:v>
+                  <c:v>29.11328125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52.789596354166697</c:v>
+                  <c:v>55.6217447916667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24.915791666666699</c:v>
+                  <c:v>33.341111111111097</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7469,11 +5339,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$57:$P$58</c:f>
+              <c:f>Sheet1!$D$253:$D$254</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Metoda MOG</c:v>
+                  <c:v>Metoda DCT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7481,7 +5351,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$N$59:$N$65</c:f>
+              <c:f>Sheet1!$B$255:$B$261</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -7510,30 +5380,105 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$59:$P$65</c:f>
+              <c:f>Sheet1!$D$255:$D$261</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>86.263981071512504</c:v>
+                  <c:v>43.188145338772998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.1932602058125</c:v>
+                  <c:v>37.526083212275701</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>181.01076035804101</c:v>
+                  <c:v>183.35071634234799</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>63.4836854878696</c:v>
+                  <c:v>34.174657921519803</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.11328125</c:v>
+                  <c:v>70.76953125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55.6217447916667</c:v>
+                  <c:v>47.315195312500002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.341111111111097</c:v>
+                  <c:v>84.560569444444397</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$253:$E$254</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Metoda Hadamard</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$255:$B$261</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>clip_01.mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>clip_02.mpg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>clip_03.mpg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clip_04.mpg</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>fountain.mpg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>highway.mpg</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>pedestrians.mpg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$255:$E$261</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43.186792682608598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.505075722649003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>183.34579284788501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.360867787646001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.773565779999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47.859283854166698</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>84.545694444444507</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7548,20 +5493,40 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="120008064"/>
-        <c:axId val="120128640"/>
+        <c:axId val="155701248"/>
+        <c:axId val="155931776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="120008064"/>
+        <c:axId val="155701248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Sekwencja</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120128640"/>
+        <c:crossAx val="155931776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7569,24 +5534,615 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120128640"/>
+        <c:axId val="155931776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Błąd średniokwadratowy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120008064"/>
+        <c:crossAx val="155701248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$229</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Średnia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$227:$I$228</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>clip_01.mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>clip_02.mpg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>clip_03.mpg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clip_04.mpg</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>fountain.mpg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>highway.mpg</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>pedestrians.mpg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$229:$I$229</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>85.9989474508303</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.393422872502398</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>198.54944371471601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62.8719152045512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.753714622641503</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56.498554687499997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>105.04234722222201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$230</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mediana</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$227:$I$228</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>clip_01.mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>clip_02.mpg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>clip_03.mpg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clip_04.mpg</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>fountain.mpg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>highway.mpg</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>pedestrians.mpg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$230:$I$230</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>53.892113710105299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.1535982393723</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>201.54178446228701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.724114684365702</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.534389740565999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52.789596354166697</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.915791666666699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$231</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MOG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$227:$I$228</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>clip_01.mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>clip_02.mpg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>clip_03.mpg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clip_04.mpg</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>fountain.mpg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>highway.mpg</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>pedestrians.mpg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$231:$I$231</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>86.263981071512504</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.1932602058125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>181.01076035804101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63.4836854878696</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29.11328125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55.6217447916667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.341111111111097</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$232</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aproksymacja średniej</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$227:$I$228</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>clip_01.mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>clip_02.mpg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>clip_03.mpg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clip_04.mpg</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>fountain.mpg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>highway.mpg</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>pedestrians.mpg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$232:$I$232</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>64.549156655851206</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.543028384032599</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>151.619960159709</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.694773788916098</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.092158018867901</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71.376106770833303</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>67.848944444444399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$233</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DCT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$227:$I$228</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>clip_01.mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>clip_02.mpg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>clip_03.mpg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clip_04.mpg</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>fountain.mpg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>highway.mpg</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>pedestrians.mpg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$233:$I$233</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43.188145338772998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.526083212275701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>183.35071634234799</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.174657921519803</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.76953125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47.315195312500002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>84.560569444444397</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$234</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hadamard</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$227:$I$228</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>clip_01.mpg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>clip_02.mpg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>clip_03.mpg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clip_04.mpg</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>fountain.mpg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>highway.mpg</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>pedestrians.mpg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$234:$I$234</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43.186792682608598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.505075722649003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>183.34579284788501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.360867787646001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.773565779999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47.859283854166698</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>84.545694444444507</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="192054400"/>
+        <c:axId val="192056320"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="192054400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sekwencja</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="192056320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="192056320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Błąd średniokwadratowy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="192054400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -7608,14 +6164,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>324969</xdr:colOff>
-      <xdr:row>124</xdr:row>
-      <xdr:rowOff>40340</xdr:rowOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>129987</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>661146</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>67235</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7637,15 +6193,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>268940</xdr:colOff>
+      <xdr:colOff>201705</xdr:colOff>
       <xdr:row>197</xdr:row>
-      <xdr:rowOff>68355</xdr:rowOff>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1042147</xdr:colOff>
       <xdr:row>220</xdr:row>
-      <xdr:rowOff>145677</xdr:rowOff>
+      <xdr:rowOff>134471</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7699,13 +6255,13 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>448234</xdr:colOff>
       <xdr:row>178</xdr:row>
-      <xdr:rowOff>214030</xdr:rowOff>
+      <xdr:rowOff>146795</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>123264</xdr:colOff>
       <xdr:row>196</xdr:row>
-      <xdr:rowOff>179295</xdr:rowOff>
+      <xdr:rowOff>112060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7719,36 +6275,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>918880</xdr:colOff>
-      <xdr:row>224</xdr:row>
-      <xdr:rowOff>169209</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>425822</xdr:colOff>
-      <xdr:row>247</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7778,7 +6304,67 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>78440</xdr:colOff>
+      <xdr:row>253</xdr:row>
+      <xdr:rowOff>158003</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>549087</xdr:colOff>
+      <xdr:row>281</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>560294</xdr:colOff>
+      <xdr:row>225</xdr:row>
+      <xdr:rowOff>146796</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>324970</xdr:colOff>
+      <xdr:row>245</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8074,10 +6660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI245"/>
+  <dimension ref="A1:AI271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L216" sqref="L216"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11368,20 +9954,20 @@
       <c r="J57" s="6">
         <v>0.16675075461686301</v>
       </c>
-      <c r="N57" s="33" t="s">
+      <c r="N57" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="O57" s="33" t="s">
+      <c r="O57" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="P57" s="33"/>
+      <c r="P57" s="34"/>
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="N58" s="33"/>
-      <c r="O58" s="31" t="s">
+      <c r="N58" s="34"/>
+      <c r="O58" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="P58" s="31" t="s">
+      <c r="P58" s="32" t="s">
         <v>16</v>
       </c>
     </row>
@@ -11416,13 +10002,13 @@
       <c r="J59" s="2">
         <v>48.315529884567503</v>
       </c>
-      <c r="N59" s="32" t="s">
+      <c r="N59" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="O59" s="37">
+      <c r="O59" s="38">
         <v>53.892113710105299</v>
       </c>
-      <c r="P59" s="37">
+      <c r="P59" s="38">
         <v>86.263981071512504</v>
       </c>
     </row>
@@ -11454,13 +10040,13 @@
       <c r="J60">
         <v>0.99406745013439601</v>
       </c>
-      <c r="N60" s="32" t="s">
+      <c r="N60" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="O60" s="37">
+      <c r="O60" s="38">
         <v>13.1535982393723</v>
       </c>
-      <c r="P60" s="37">
+      <c r="P60" s="38">
         <v>25.1932602058125</v>
       </c>
     </row>
@@ -11492,13 +10078,13 @@
       <c r="J61">
         <v>0.91956262667559696</v>
       </c>
-      <c r="N61" s="32" t="s">
+      <c r="N61" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="O61" s="37">
+      <c r="O61" s="38">
         <v>201.54178446228701</v>
       </c>
-      <c r="P61" s="37">
+      <c r="P61" s="38">
         <v>181.01076035804101</v>
       </c>
     </row>
@@ -11530,13 +10116,13 @@
       <c r="J62">
         <v>0.72841186857923301</v>
       </c>
-      <c r="N62" s="32" t="s">
+      <c r="N62" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="O62" s="37">
+      <c r="O62" s="38">
         <v>32.724114684365702</v>
       </c>
-      <c r="P62" s="37">
+      <c r="P62" s="38">
         <v>63.4836854878696</v>
       </c>
     </row>
@@ -11568,24 +10154,24 @@
       <c r="J63">
         <v>0.46780591341260802</v>
       </c>
-      <c r="N63" s="32" t="s">
+      <c r="N63" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="O63" s="37">
+      <c r="O63" s="38">
         <v>36.534389740565999</v>
       </c>
-      <c r="P63" s="37">
+      <c r="P63" s="38">
         <v>29.11328125</v>
       </c>
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="N64" s="32" t="s">
+      <c r="N64" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="O64" s="37">
+      <c r="O64" s="38">
         <v>52.789596354166697</v>
       </c>
-      <c r="P64" s="37">
+      <c r="P64" s="38">
         <v>55.6217447916667</v>
       </c>
     </row>
@@ -11620,13 +10206,13 @@
       <c r="J65" s="2">
         <v>151.619960159709</v>
       </c>
-      <c r="N65" s="32" t="s">
+      <c r="N65" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="O65" s="37">
+      <c r="O65" s="38">
         <v>24.915791666666699</v>
       </c>
-      <c r="P65" s="37">
+      <c r="P65" s="38">
         <v>33.341111111111097</v>
       </c>
     </row>
@@ -14759,404 +13345,564 @@
       </c>
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B227" s="34" t="s">
+      <c r="B227" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C227" s="34" t="s">
+      <c r="C227" s="35"/>
+      <c r="D227" s="35"/>
+      <c r="E227" s="35"/>
+      <c r="F227" s="35"/>
+      <c r="G227" s="35"/>
+      <c r="H227" s="35"/>
+      <c r="I227" s="35"/>
+    </row>
+    <row r="228" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B228" s="35"/>
+      <c r="C228" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D228" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E228" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="F228" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="G228" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="H228" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="I228" s="36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="229" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B229" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C229" s="38">
+        <v>85.9989474508303</v>
+      </c>
+      <c r="D229" s="38">
+        <v>38.393422872502398</v>
+      </c>
+      <c r="E229" s="38">
+        <v>198.54944371471601</v>
+      </c>
+      <c r="F229" s="38">
+        <v>62.8719152045512</v>
+      </c>
+      <c r="G229" s="38">
+        <v>37.753714622641503</v>
+      </c>
+      <c r="H229" s="38">
+        <v>56.498554687499997</v>
+      </c>
+      <c r="I229" s="38">
+        <v>105.04234722222201</v>
+      </c>
+    </row>
+    <row r="230" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B230" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C230" s="38">
+        <v>53.892113710105299</v>
+      </c>
+      <c r="D230" s="38">
+        <v>13.1535982393723</v>
+      </c>
+      <c r="E230" s="38">
+        <v>201.54178446228701</v>
+      </c>
+      <c r="F230" s="38">
+        <v>32.724114684365702</v>
+      </c>
+      <c r="G230" s="38">
+        <v>36.534389740565999</v>
+      </c>
+      <c r="H230" s="38">
+        <v>52.789596354166697</v>
+      </c>
+      <c r="I230" s="38">
+        <v>24.915791666666699</v>
+      </c>
+    </row>
+    <row r="231" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B231" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C231" s="38">
+        <v>86.263981071512504</v>
+      </c>
+      <c r="D231" s="38">
+        <v>25.1932602058125</v>
+      </c>
+      <c r="E231" s="38">
+        <v>181.01076035804101</v>
+      </c>
+      <c r="F231" s="38">
+        <v>63.4836854878696</v>
+      </c>
+      <c r="G231" s="38">
+        <v>29.11328125</v>
+      </c>
+      <c r="H231" s="38">
+        <v>55.6217447916667</v>
+      </c>
+      <c r="I231" s="38">
+        <v>33.341111111111097</v>
+      </c>
+    </row>
+    <row r="232" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B232" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C232" s="38">
+        <v>64.549156655851206</v>
+      </c>
+      <c r="D232" s="38">
+        <v>29.543028384032599</v>
+      </c>
+      <c r="E232" s="38">
+        <v>151.619960159709</v>
+      </c>
+      <c r="F232" s="38">
+        <v>21.694773788916098</v>
+      </c>
+      <c r="G232" s="38">
+        <v>13.092158018867901</v>
+      </c>
+      <c r="H232" s="38">
+        <v>71.376106770833303</v>
+      </c>
+      <c r="I232" s="38">
+        <v>67.848944444444399</v>
+      </c>
+    </row>
+    <row r="233" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B233" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C233" s="38">
+        <v>43.188145338772998</v>
+      </c>
+      <c r="D233" s="38">
+        <v>37.526083212275701</v>
+      </c>
+      <c r="E233" s="38">
+        <v>183.35071634234799</v>
+      </c>
+      <c r="F233" s="38">
+        <v>34.174657921519803</v>
+      </c>
+      <c r="G233" s="38">
+        <v>70.76953125</v>
+      </c>
+      <c r="H233" s="38">
+        <v>47.315195312500002</v>
+      </c>
+      <c r="I233" s="38">
+        <v>84.560569444444397</v>
+      </c>
+    </row>
+    <row r="234" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B234" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C234" s="38">
+        <v>43.186792682608598</v>
+      </c>
+      <c r="D234" s="38">
+        <v>37.505075722649003</v>
+      </c>
+      <c r="E234" s="38">
+        <v>183.34579284788501</v>
+      </c>
+      <c r="F234" s="38">
+        <v>34.360867787646001</v>
+      </c>
+      <c r="G234" s="38">
+        <v>70.773565779999998</v>
+      </c>
+      <c r="H234" s="38">
+        <v>47.859283854166698</v>
+      </c>
+      <c r="I234" s="38">
+        <v>84.545694444444507</v>
+      </c>
+    </row>
+    <row r="237" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C237" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D227" s="34"/>
-      <c r="E227" s="34"/>
-      <c r="F227" s="34"/>
-      <c r="G227" s="34"/>
-      <c r="H227" s="34"/>
-      <c r="I227" s="34"/>
-    </row>
-    <row r="228" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B228" s="34"/>
-      <c r="C228" s="35" t="s">
+      <c r="D237" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="E237" s="49"/>
+      <c r="F237" s="49"/>
+      <c r="G237" s="49"/>
+      <c r="H237" s="49"/>
+      <c r="I237" s="50"/>
+    </row>
+    <row r="238" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B238" s="40"/>
+      <c r="C238" s="47"/>
+      <c r="D238" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="E238" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="F238" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G238" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H238" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="I238" s="44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="239" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B239" s="41"/>
+      <c r="C239" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D228" s="35" t="s">
+      <c r="D239" s="38">
+        <v>85.9989474508303</v>
+      </c>
+      <c r="E239" s="38">
+        <v>53.892113710105299</v>
+      </c>
+      <c r="F239" s="38">
+        <v>86.263981071512504</v>
+      </c>
+      <c r="G239" s="38">
+        <v>64.549156655851206</v>
+      </c>
+      <c r="H239" s="38">
+        <v>43.188145338772998</v>
+      </c>
+      <c r="I239" s="38">
+        <v>43.186792682608598</v>
+      </c>
+    </row>
+    <row r="240" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B240" s="42"/>
+      <c r="C240" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E228" s="35" t="s">
+      <c r="D240" s="38">
+        <v>38.393422872502398</v>
+      </c>
+      <c r="E240" s="38">
+        <v>13.1535982393723</v>
+      </c>
+      <c r="F240" s="38">
+        <v>25.1932602058125</v>
+      </c>
+      <c r="G240" s="38">
+        <v>29.543028384032599</v>
+      </c>
+      <c r="H240" s="38">
+        <v>37.526083212275701</v>
+      </c>
+      <c r="I240" s="38">
+        <v>37.505075722649003</v>
+      </c>
+    </row>
+    <row r="241" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B241" s="42"/>
+      <c r="C241" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F228" s="35" t="s">
+      <c r="D241" s="38">
+        <v>198.54944371471601</v>
+      </c>
+      <c r="E241" s="38">
+        <v>201.54178446228701</v>
+      </c>
+      <c r="F241" s="38">
+        <v>181.01076035804101</v>
+      </c>
+      <c r="G241" s="38">
+        <v>151.619960159709</v>
+      </c>
+      <c r="H241" s="38">
+        <v>183.35071634234799</v>
+      </c>
+      <c r="I241" s="38">
+        <v>183.34579284788501</v>
+      </c>
+    </row>
+    <row r="242" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B242" s="42"/>
+      <c r="C242" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="G228" s="35" t="s">
+      <c r="D242" s="38">
+        <v>62.8719152045512</v>
+      </c>
+      <c r="E242" s="38">
+        <v>32.724114684365702</v>
+      </c>
+      <c r="F242" s="38">
+        <v>63.4836854878696</v>
+      </c>
+      <c r="G242" s="38">
+        <v>21.694773788916098</v>
+      </c>
+      <c r="H242" s="38">
+        <v>34.174657921519803</v>
+      </c>
+      <c r="I242" s="38">
+        <v>34.360867787646001</v>
+      </c>
+    </row>
+    <row r="243" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B243" s="42"/>
+      <c r="C243" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="H228" s="35" t="s">
+      <c r="D243" s="38">
+        <v>37.753714622641503</v>
+      </c>
+      <c r="E243" s="38">
+        <v>36.534389740565999</v>
+      </c>
+      <c r="F243" s="38">
+        <v>29.11328125</v>
+      </c>
+      <c r="G243" s="38">
+        <v>13.092158018867901</v>
+      </c>
+      <c r="H243" s="38">
+        <v>70.76953125</v>
+      </c>
+      <c r="I243" s="38">
+        <v>70.773565779999998</v>
+      </c>
+    </row>
+    <row r="244" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B244" s="42"/>
+      <c r="C244" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="I228" s="35" t="s">
+      <c r="D244" s="38">
+        <v>56.498554687499997</v>
+      </c>
+      <c r="E244" s="38">
+        <v>52.789596354166697</v>
+      </c>
+      <c r="F244" s="38">
+        <v>55.6217447916667</v>
+      </c>
+      <c r="G244" s="38">
+        <v>71.376106770833303</v>
+      </c>
+      <c r="H244" s="38">
+        <v>47.315195312500002</v>
+      </c>
+      <c r="I244" s="38">
+        <v>47.859283854166698</v>
+      </c>
+    </row>
+    <row r="245" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B245" s="43"/>
+      <c r="C245" s="44" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="229" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B229" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C229" s="37">
-        <v>85.9989474508303</v>
-      </c>
-      <c r="D229" s="37">
-        <v>38.393422872502398</v>
-      </c>
-      <c r="E229" s="37">
-        <v>198.54944371471601</v>
-      </c>
-      <c r="F229" s="37">
-        <v>62.8719152045512</v>
-      </c>
-      <c r="G229" s="37">
-        <v>37.753714622641503</v>
-      </c>
-      <c r="H229" s="37">
-        <v>56.498554687499997</v>
-      </c>
-      <c r="I229" s="37">
+      <c r="D245" s="38">
         <v>105.04234722222201</v>
       </c>
-    </row>
-    <row r="230" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B230" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="C230" s="37">
-        <v>53.892113710105299</v>
-      </c>
-      <c r="D230" s="37">
-        <v>13.1535982393723</v>
-      </c>
-      <c r="E230" s="37">
-        <v>201.54178446228701</v>
-      </c>
-      <c r="F230" s="37">
-        <v>32.724114684365702</v>
-      </c>
-      <c r="G230" s="37">
-        <v>36.534389740565999</v>
-      </c>
-      <c r="H230" s="37">
-        <v>52.789596354166697</v>
-      </c>
-      <c r="I230" s="37">
+      <c r="E245" s="38">
         <v>24.915791666666699</v>
       </c>
-    </row>
-    <row r="231" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B231" s="36" t="s">
+      <c r="F245" s="38">
+        <v>33.341111111111097</v>
+      </c>
+      <c r="G245" s="38">
+        <v>67.848944444444399</v>
+      </c>
+      <c r="H245" s="38">
+        <v>84.560569444444397</v>
+      </c>
+      <c r="I245" s="38">
+        <v>84.545694444444507</v>
+      </c>
+    </row>
+    <row r="253" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B253" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C253" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="D253" s="54"/>
+      <c r="E253" s="54"/>
+      <c r="F253" s="51"/>
+      <c r="G253" s="51"/>
+      <c r="H253" s="52"/>
+    </row>
+    <row r="254" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B254" s="54"/>
+      <c r="C254" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C231" s="37">
+      <c r="D254" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E254" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="F254" s="53"/>
+    </row>
+    <row r="255" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B255" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C255" s="38">
         <v>86.263981071512504</v>
       </c>
-      <c r="D231" s="37">
+      <c r="D255" s="38">
+        <v>43.188145338772998</v>
+      </c>
+      <c r="E255" s="38">
+        <v>43.186792682608598</v>
+      </c>
+    </row>
+    <row r="256" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B256" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C256" s="38">
         <v>25.1932602058125</v>
       </c>
-      <c r="E231" s="37">
+      <c r="D256" s="38">
+        <v>37.526083212275701</v>
+      </c>
+      <c r="E256" s="38">
+        <v>37.505075722649003</v>
+      </c>
+    </row>
+    <row r="257" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B257" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C257" s="38">
         <v>181.01076035804101</v>
       </c>
-      <c r="F231" s="37">
+      <c r="D257" s="38">
+        <v>183.35071634234799</v>
+      </c>
+      <c r="E257" s="38">
+        <v>183.34579284788501</v>
+      </c>
+    </row>
+    <row r="258" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B258" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C258" s="38">
         <v>63.4836854878696</v>
       </c>
-      <c r="G231" s="37">
+      <c r="D258" s="38">
+        <v>34.174657921519803</v>
+      </c>
+      <c r="E258" s="38">
+        <v>34.360867787646001</v>
+      </c>
+    </row>
+    <row r="259" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B259" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C259" s="38">
         <v>29.11328125</v>
       </c>
-      <c r="H231" s="37">
+      <c r="D259" s="38">
+        <v>70.76953125</v>
+      </c>
+      <c r="E259" s="38">
+        <v>70.773565779999998</v>
+      </c>
+    </row>
+    <row r="260" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B260" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C260" s="38">
         <v>55.6217447916667</v>
       </c>
-      <c r="I231" s="37">
+      <c r="D260" s="38">
+        <v>47.315195312500002</v>
+      </c>
+      <c r="E260" s="38">
+        <v>47.859283854166698</v>
+      </c>
+    </row>
+    <row r="261" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B261" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C261" s="38">
         <v>33.341111111111097</v>
       </c>
-    </row>
-    <row r="232" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B232" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C232" s="37">
-        <v>64.549156655851206</v>
-      </c>
-      <c r="D232" s="37">
-        <v>29.543028384032599</v>
-      </c>
-      <c r="E232" s="37">
-        <v>151.619960159709</v>
-      </c>
-      <c r="F232" s="37">
-        <v>21.694773788916098</v>
-      </c>
-      <c r="G232" s="37">
-        <v>13.092158018867901</v>
-      </c>
-      <c r="H232" s="37">
-        <v>71.376106770833303</v>
-      </c>
-      <c r="I232" s="37">
-        <v>67.848944444444399</v>
-      </c>
-    </row>
-    <row r="233" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B233" s="35" t="s">
+      <c r="D261" s="38">
+        <v>84.560569444444397</v>
+      </c>
+      <c r="E261" s="38">
+        <v>84.545694444444507</v>
+      </c>
+    </row>
+    <row r="264" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B264" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C264" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D264" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C233" s="37">
-        <v>43.188145338772998</v>
-      </c>
-      <c r="D233" s="37">
-        <v>37.526083212275701</v>
-      </c>
-      <c r="E233" s="37">
-        <v>183.35071634234799</v>
-      </c>
-      <c r="F233" s="37">
-        <v>34.174657921519803</v>
-      </c>
-      <c r="G233" s="37">
-        <v>70.76953125</v>
-      </c>
-      <c r="H233" s="37">
-        <v>47.315195312500002</v>
-      </c>
-      <c r="I233" s="37">
-        <v>84.560569444444397</v>
-      </c>
-    </row>
-    <row r="234" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B234" s="35" t="s">
+      <c r="E264" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C234" s="37">
-        <v>43.186792682608598</v>
-      </c>
-      <c r="D234" s="37">
-        <v>37.505075722649003</v>
-      </c>
-      <c r="E234" s="37">
-        <v>183.34579284788501</v>
-      </c>
-      <c r="F234" s="37">
-        <v>34.360867787646001</v>
-      </c>
-      <c r="G234" s="37">
-        <v>70.773565779999998</v>
-      </c>
-      <c r="H234" s="37">
-        <v>47.859283854166698</v>
-      </c>
-      <c r="I234" s="37">
-        <v>84.545694444444507</v>
-      </c>
-    </row>
-    <row r="237" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C237" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="D237" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="E237" s="48"/>
-      <c r="F237" s="48"/>
-      <c r="G237" s="48"/>
-      <c r="H237" s="48"/>
-      <c r="I237" s="49"/>
-    </row>
-    <row r="238" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B238" s="39"/>
-      <c r="C238" s="46"/>
-      <c r="D238" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="E238" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="F238" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="G238" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="H238" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="I238" s="43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="239" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B239" s="40"/>
-      <c r="C239" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="D239" s="37">
-        <v>85.9989474508303</v>
-      </c>
-      <c r="E239" s="37">
-        <v>53.892113710105299</v>
-      </c>
-      <c r="F239" s="37">
-        <v>86.263981071512504</v>
-      </c>
-      <c r="G239" s="37">
-        <v>64.549156655851206</v>
-      </c>
-      <c r="H239" s="37">
-        <v>43.188145338772998</v>
-      </c>
-      <c r="I239" s="37">
-        <v>43.186792682608598</v>
-      </c>
-    </row>
-    <row r="240" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B240" s="41"/>
-      <c r="C240" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D240" s="37">
-        <v>38.393422872502398</v>
-      </c>
-      <c r="E240" s="37">
-        <v>13.1535982393723</v>
-      </c>
-      <c r="F240" s="37">
-        <v>25.1932602058125</v>
-      </c>
-      <c r="G240" s="37">
-        <v>29.543028384032599</v>
-      </c>
-      <c r="H240" s="37">
-        <v>37.526083212275701</v>
-      </c>
-      <c r="I240" s="37">
-        <v>37.505075722649003</v>
-      </c>
-    </row>
-    <row r="241" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B241" s="41"/>
-      <c r="C241" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="D241" s="37">
-        <v>198.54944371471601</v>
-      </c>
-      <c r="E241" s="37">
-        <v>201.54178446228701</v>
-      </c>
-      <c r="F241" s="37">
-        <v>181.01076035804101</v>
-      </c>
-      <c r="G241" s="37">
-        <v>151.619960159709</v>
-      </c>
-      <c r="H241" s="37">
-        <v>183.35071634234799</v>
-      </c>
-      <c r="I241" s="37">
-        <v>183.34579284788501</v>
-      </c>
-    </row>
-    <row r="242" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B242" s="41"/>
-      <c r="C242" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="D242" s="37">
-        <v>62.8719152045512</v>
-      </c>
-      <c r="E242" s="37">
-        <v>32.724114684365702</v>
-      </c>
-      <c r="F242" s="37">
-        <v>63.4836854878696</v>
-      </c>
-      <c r="G242" s="37">
-        <v>21.694773788916098</v>
-      </c>
-      <c r="H242" s="37">
-        <v>34.174657921519803</v>
-      </c>
-      <c r="I242" s="37">
-        <v>34.360867787646001</v>
-      </c>
-    </row>
-    <row r="243" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B243" s="41"/>
-      <c r="C243" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="D243" s="37">
-        <v>37.753714622641503</v>
-      </c>
-      <c r="E243" s="37">
-        <v>36.534389740565999</v>
-      </c>
-      <c r="F243" s="37">
-        <v>29.11328125</v>
-      </c>
-      <c r="G243" s="37">
-        <v>13.092158018867901</v>
-      </c>
-      <c r="H243" s="37">
-        <v>70.76953125</v>
-      </c>
-      <c r="I243" s="37">
-        <v>70.773565779999998</v>
-      </c>
-    </row>
-    <row r="244" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B244" s="41"/>
-      <c r="C244" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="D244" s="37">
-        <v>56.498554687499997</v>
-      </c>
-      <c r="E244" s="37">
-        <v>52.789596354166697</v>
-      </c>
-      <c r="F244" s="37">
-        <v>55.6217447916667</v>
-      </c>
-      <c r="G244" s="37">
-        <v>71.376106770833303</v>
-      </c>
-      <c r="H244" s="37">
-        <v>47.315195312500002</v>
-      </c>
-      <c r="I244" s="37">
-        <v>47.859283854166698</v>
-      </c>
-    </row>
-    <row r="245" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B245" s="42"/>
-      <c r="C245" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="D245" s="37">
-        <v>105.04234722222201</v>
-      </c>
-      <c r="E245" s="37">
-        <v>24.915791666666699</v>
-      </c>
-      <c r="F245" s="37">
-        <v>33.341111111111097</v>
-      </c>
-      <c r="G245" s="37">
-        <v>67.848944444444399</v>
-      </c>
-      <c r="H245" s="37">
-        <v>84.560569444444397</v>
-      </c>
-      <c r="I245" s="37">
-        <v>84.545694444444507</v>
-      </c>
+      <c r="F264" s="23"/>
+    </row>
+    <row r="265" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F265" s="6"/>
+    </row>
+    <row r="266" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F266" s="2"/>
+    </row>
+    <row r="267" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F267" s="2"/>
+    </row>
+    <row r="268" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F268" s="2"/>
+    </row>
+    <row r="269" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F269" s="2"/>
+    </row>
+    <row r="270" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F270" s="2"/>
+    </row>
+    <row r="271" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F271" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="52">
+    <mergeCell ref="B253:B254"/>
+    <mergeCell ref="C253:E253"/>
     <mergeCell ref="C237:C238"/>
     <mergeCell ref="D237:I237"/>
     <mergeCell ref="N57:N58"/>

</xml_diff>